<commit_message>
updated work in progress code, and strated creating final pipeline for analysis
</commit_message>
<xml_diff>
--- a/Environmental_datasets/Environmental databases.xlsx
+++ b/Environmental_datasets/Environmental databases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmersonEmmerson/Documents/Master's/C_forecasting_NL/Environmental_datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D554514-687D-544F-A389-A6834DF1F6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609B581D-3843-974D-A485-66FD6A828631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="17500" activeTab="4" xr2:uid="{9EEE58CE-D387-B14C-ABB0-8398CF6D0276}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="17500" activeTab="3" xr2:uid="{9EEE58CE-D387-B14C-ABB0-8398CF6D0276}"/>
   </bookViews>
   <sheets>
     <sheet name="Databases" sheetId="1" r:id="rId1"/>
@@ -4366,9 +4366,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4406,7 +4406,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4512,7 +4512,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4654,7 +4654,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4749,7 +4749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCEAFAD-3713-EF4E-AB7A-ABE53C4DA4AA}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="B6" zoomScale="125" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -5510,8 +5510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1194E792-5E87-AD45-9D02-CDD373EDE6D4}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -5999,9 +5999,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5651BE44-E033-A741-8310-2B47115ACEA4}">
   <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E12" sqref="E12"/>
+      <selection pane="topRight" activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7718,7 +7718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F487AF0-5C57-A443-979D-79FDCB7DF6BB}">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="88" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="88" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B11" sqref="B11"/>
     </sheetView>
@@ -9150,15 +9150,16 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="75" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B16" sqref="B16"/>
+      <selection pane="topRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="31.83203125" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="26.6640625" style="30" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="30" customWidth="1"/>
+    <col min="3" max="4" width="26.6640625" style="30" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" style="30" customWidth="1"/>
     <col min="6" max="10" width="10.83203125" style="30" customWidth="1"/>
     <col min="11" max="11" width="48.5" style="30" customWidth="1"/>

</xml_diff>